<commit_message>
Updated Codes for Birthplaces
</commit_message>
<xml_diff>
--- a/Data/CodesForBirthplace.xlsx
+++ b/Data/CodesForBirthplace.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GP\Desktop\MEGHA\SemII\JSM-ASA Challenge\JSM-project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B991EC4-6BA6-4EAD-991D-5340753E8594}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B36727-6030-4EE5-B7AB-B148892A1151}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Code</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Mexico, Central America, South America</t>
   </si>
   <si>
-    <t>Russia/successor states to soviet union</t>
-  </si>
-  <si>
     <t>China, Hong Kong, Taiwan</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
     <t>Not reported</t>
   </si>
   <si>
-    <t>Europe, Central Asia, Transcaucasia</t>
-  </si>
-  <si>
     <t>Combine NYC and US(outside NYC)</t>
   </si>
   <si>
@@ -88,10 +82,13 @@
     <t>Combine Canada with All Other Countries</t>
   </si>
   <si>
-    <t>Combine Europe, Other European Countries, Baltic States, Central Asia and Transcaucasia - Baltic states include Estonia, Latvia and Lithuania | Central Asia includes Kazakhstan, Krygyztan, Tajikistan, Turkmenistan, and Uzbekistan | Transcaucasia includes Armenia, Azerbaijan, and Georgia</t>
-  </si>
-  <si>
     <t>Directions</t>
+  </si>
+  <si>
+    <t>Europe, Russia, Central Asia, Transcaucasia</t>
+  </si>
+  <si>
+    <t>Combine Europe, Other European Countries, Russia, Baltic States, Central Asia and Transcaucasia - Baltic states include Estonia, Latvia and Lithuania | Central Asia includes Kazakhstan, Krygyztan, Tajikistan, Turkmenistan, and Uzbekistan | Transcaucasia includes Armenia, Azerbaijan, and Georgia</t>
   </si>
 </sst>
 </file>
@@ -488,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFFD2287-C539-447C-805D-1DF9BAAA5FA6}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C11" sqref="C10:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -511,7 +508,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D1" s="2"/>
     </row>
@@ -523,7 +520,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -561,15 +558,15 @@
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="71.25" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>22</v>
@@ -577,7 +574,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>7</v>
@@ -586,7 +583,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>8</v>
@@ -595,27 +592,27 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>11</v>
@@ -624,7 +621,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>12</v>
@@ -633,7 +630,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>13</v>
@@ -642,32 +639,23 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
-        <v>98</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="4"/>
+      <c r="C16" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>